<commit_message>
Change date in db
</commit_message>
<xml_diff>
--- a/data_base/Data_base.xlsx
+++ b/data_base/Data_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aubkhonabdullaev/Projects/WebProject1/data_base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1F462D-6082-D34B-88C5-147C751FE9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3F2EE3-53C7-ED4D-9735-34E8A0EA23B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{BD201720-335B-A143-861E-5430A88ECA3B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{BD201720-335B-A143-861E-5430A88ECA3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Product</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>real</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>birth_date</t>
+  </si>
+  <si>
+    <t>start_date</t>
   </si>
 </sst>
 </file>
@@ -637,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CED8707-B9E1-D34E-A2A7-865394EE6D15}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="195" zoomScaleNormal="195" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -700,7 +709,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -720,7 +729,7 @@
         <v>8</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -740,7 +749,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -760,7 +769,7 @@
         <v>9</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -769,6 +778,32 @@
       </c>
       <c r="B7" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>